<commit_message>
updtaed data dict. filling RFM datatypes
</commit_message>
<xml_diff>
--- a/Neural_Nexus_Customer_Segmentation_Data_Dictionary.xlsx
+++ b/Neural_Nexus_Customer_Segmentation_Data_Dictionary.xlsx
@@ -1,42 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manwarsadat\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654858B9-EDBB-4C10-A7B3-9A1C0DC1F955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C8B4FF16-426B-42DA-BE68-D2E72EF359E5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
   <si>
     <t>Feature Name</t>
   </si>
@@ -111,13 +89,79 @@
   </si>
   <si>
     <t>Float</t>
+  </si>
+  <si>
+    <t>Recency</t>
+  </si>
+  <si>
+    <t>Measures how recently a customer made a purchase. The more recent the transaction, the more likely the customer is to respond to future promotions.</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Measures how often a customer makes a purchase within a given time period. Frequent buyers are generally more engaged and loyal.</t>
+  </si>
+  <si>
+    <t>Monetary</t>
+  </si>
+  <si>
+    <t>Measures how much a customer spends. High-spending customers are more valuable and should be treated accordingly.</t>
+  </si>
+  <si>
+    <t>TotalQuantity</t>
+  </si>
+  <si>
+    <t>TotalPrice = Quantity * UnitPrice</t>
+  </si>
+  <si>
+    <t>AvgQuantity</t>
+  </si>
+  <si>
+    <t>average quantity of purchases</t>
+  </si>
+  <si>
+    <t>AvgSpend</t>
+  </si>
+  <si>
+    <t>average spending of customers</t>
+  </si>
+  <si>
+    <t>ProductDiversity</t>
+  </si>
+  <si>
+    <t>displays the diversity of the products that are purchased</t>
+  </si>
+  <si>
+    <t>R_Score</t>
+  </si>
+  <si>
+    <t>scores 1-5 for Recency</t>
+  </si>
+  <si>
+    <t>F_Score</t>
+  </si>
+  <si>
+    <t>scores 1-5 for Frequency</t>
+  </si>
+  <si>
+    <t>M_Score</t>
+  </si>
+  <si>
+    <t>scores 1-5 for Monetary</t>
+  </si>
+  <si>
+    <t>RFM_Score</t>
+  </si>
+  <si>
+    <t>scores 1-5 for sum of Recency, Frequency and Monetary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,7 +190,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -160,9 +205,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -211,7 +253,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -263,7 +305,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -477,151 +519,305 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AAC343-2BF7-41E1-8048-684947AAF263}">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="31.7265625" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" customWidth="1"/>
-    <col min="3" max="3" width="71.7265625" customWidth="1"/>
-    <col min="4" max="4" width="25.26953125" customWidth="1"/>
+    <col min="1" max="1" width="31.69921875" customWidth="1"/>
+    <col min="2" max="2" width="18.796875" customWidth="1"/>
+    <col min="3" max="3" width="71.69921875" customWidth="1"/>
+    <col min="4" max="4" width="25.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="27.6">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" ht="27.6">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>